<commit_message>
ECP-1125: filters empty turnover comments
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated_minute.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated_minute.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657F7E57-2A8D-5E4B-928E-16B203237389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F0A8C2-D4EF-8941-8BAD-64AE20F62B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33820" windowHeight="20300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,12 +152,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -285,12 +291,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="114">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -745,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -885,32 +895,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+    <row r="4" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>43689</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>43709</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4">
+      <c r="E4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="8">
         <v>33255</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="8">
         <v>1101</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1542,35 +1552,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="3">
-        <v>41791</v>
-      </c>
-      <c r="D25" s="3">
+      <c r="C25" s="6">
+        <v>41791</v>
+      </c>
+      <c r="D25" s="6">
         <v>42856</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G25" s="4">
-        <v>0</v>
-      </c>
-      <c r="H25" s="4">
-        <v>0</v>
-      </c>
-      <c r="J25" s="4">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="E25" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>